<commit_message>
Added normalization to WT
</commit_message>
<xml_diff>
--- a/Datasets/20007368/raw_data/0909777106_0909777106S.xlsx
+++ b/Datasets/20007368/raw_data/0909777106_0909777106S.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gradstudent\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="22380" windowHeight="10780"/>
   </bookViews>
   <sheets>
     <sheet name="0909777106_0909777106S" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>YHR014W</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>(0.3)</t>
+  </si>
+  <si>
+    <t>BY4743</t>
+  </si>
+  <si>
+    <t>(0.32)</t>
   </si>
 </sst>
 </file>
@@ -786,7 +792,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,7 +827,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -998,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1006,544 +1012,581 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1">
+        <v>0.08</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1">
+        <v>0.05</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1">
+        <v>0.06</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1">
+        <v>0.03</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>0.74</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1">
+      <c r="E2">
         <v>0.8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1">
+      <c r="G2">
         <v>0.84</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1">
+      <c r="I2">
         <v>0.64</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1">
+      <c r="K2">
         <v>3.02</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>0.9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>0.9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>0.6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I2">
+      <c r="I3">
         <v>0.5</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K2">
+      <c r="K3">
         <v>2.9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1.02</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>0.94</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <v>0.98</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>0.46</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K3">
+      <c r="K4">
         <v>3.4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.98</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>0.98</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G4">
+      <c r="G5">
         <v>0.71</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I4">
-        <v>0.27</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4">
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>0.9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>0.88</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>0.78</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
       <c r="I5">
+        <v>0.27</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>0.88</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>0.78</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6">
         <v>0.18</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <v>2.74</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>0.99</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>0.93</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>0.62</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>0.13</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>2.67</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>0.96</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.98</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0.9</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>0.09</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>2.93</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>0.99</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8">
-        <v>0.83</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8">
-        <v>0.06</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8">
-        <v>2.97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9">
-        <v>0.96</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>0.91</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G9">
-        <v>0.71</v>
+        <v>0.83</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I9">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="K9">
-        <v>2.62</v>
+        <v>2.97</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>0.84</v>
+        <v>0.96</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10">
-        <v>0.94</v>
+        <v>0.91</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G10">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I10">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="K10">
-        <v>2.5299999999999998</v>
+        <v>2.62</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>0.92</v>
+        <v>0.84</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E11">
-        <v>0.85</v>
+        <v>0.94</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G11">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="I11">
         <v>0.02</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>0.92</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>0.85</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>0.71</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12">
+        <v>0.02</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>0.89</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>0.87</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12">
-        <v>0.01</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12">
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>0.94</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13">
-        <v>0.91</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G13">
-        <v>0.63</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="I13">
         <v>0.01</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="K13">
-        <v>2.4900000000000002</v>
+        <v>2.33</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14">
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>0.91</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14">
-        <v>0.84</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G14">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="I14">
         <v>0.01</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="K14">
-        <v>2.46</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15">
-        <v>0.92</v>
+        <v>0.98</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E15">
-        <v>0.94</v>
+        <v>0.84</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G15">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="I15">
         <v>0.01</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>0.92</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16">
+        <v>0.94</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16">
+        <v>0.59</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16">
+        <v>0.01</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K15">
+      <c r="K16">
         <v>2.4500000000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>